<commit_message>
ABC Base Punto Venta
</commit_message>
<xml_diff>
--- a/Scripts_R110_Catalogos/LIQ19_R110_01.b_CI_Punto_Venta.XLSX
+++ b/Scripts_R110_Catalogos/LIQ19_R110_01.b_CI_Punto_Venta.XLSX
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="134">
   <si>
     <t>K_PUNTO_VENTA</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>C_PUNTO_VENTA</t>
   </si>
 </sst>
 </file>
@@ -821,13 +824,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S51"/>
+  <dimension ref="B2:T51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -836,21 +839,22 @@
     <col min="2" max="2" width="13.1328125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="84" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.86328125" customWidth="1"/>
-    <col min="17" max="17" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.9296875" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="84" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.86328125" customWidth="1"/>
+    <col min="18" max="18" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -861,26 +865,29 @@
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="3"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -891,32 +898,32 @@
         <f>LEFT(C3,3)</f>
         <v>BE2</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
       </c>
       <c r="I3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K3" s="3" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, ",B3,", '",C3,"', '",D3,"', ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 1, 'BE201', 'BE2', 1, 0, 1, BIOGAS, ABC123, N/A; </v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L3" s="3" t="str">
+        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, ",B3,", '",C3,"', '",D3,"','",E3,"', ",F3,", ",G3,", ",H3,", '",I3,"', '",J3,"', '",K3,"'; ")</f>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 1, 'BE201', 'BE2','', 1, 0, 1, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -924,35 +931,35 @@
         <v>20</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D50" si="0">LEFT(C4,3)</f>
+        <f t="shared" ref="D4:E50" si="0">LEFT(C4,3)</f>
         <v>C13</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9">
         <v>3</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="K4" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="3" t="str">
-        <f t="shared" ref="K4:K50" si="1">CONCATENATE("EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, ",B4,", '",C4,"', '",D4,"', ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 2, 'C133', 'C13', 2, 1, 3, BIOGAS, BCD456, N/A; </v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="S4" s="3"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L4" s="3" t="str">
+        <f t="shared" ref="L4:L50" si="1">CONCATENATE("EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, ",B4,", '",C4,"', '",D4,"','",E4,"', ",F4,", ",G4,", ",H4,", '",I4,"', '",J4,"', '",K4,"'; ")</f>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 2, 'C133', 'C13','', 2, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -963,32 +970,32 @@
         <f t="shared" si="0"/>
         <v>BG2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
         <v>2</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="3" t="str">
+      <c r="L5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 3, 'BG29', 'BG2', 3, 1, 2, MARKETING, N/A, Av. Independencia; </v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="S5" s="3"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 3, 'BG29', 'BG2','', 3, 1, 2, 'MARKETING', 'N/A', 'Av. Independencia'; </v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -999,33 +1006,33 @@
         <f t="shared" si="0"/>
         <v>BE0</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
         <v>3</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="I6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K6" s="3" t="str">
+      <c r="L6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 4, 'BE03', 'BE0', 4, 0, 3, BIOGAS, EDF678, N/A; </v>
-      </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="10"/>
-      <c r="S6" s="3"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 4, 'BE03', 'BE0','', 4, 0, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="10"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -1036,31 +1043,31 @@
         <f t="shared" si="0"/>
         <v>BE0</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9">
         <v>3</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="3" t="str">
+      <c r="L7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 5, 'BE04', 'BE0', 5, 1, 3, BIOGAS, ABC123, N/A; </v>
-      </c>
-      <c r="P7" s="7"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 5, 'BE04', 'BE0','', 5, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1071,35 +1078,35 @@
         <f t="shared" si="0"/>
         <v>BG0</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
         <v>3</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K8" s="3" t="str">
+      <c r="L8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 6, 'BG03', 'BG0', 6, 1, 3, BIOGAS, BCD456, N/A; </v>
-      </c>
-      <c r="L8" s="2"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 6, 'BG03', 'BG0','', 6, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="7"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <v>8</v>
       </c>
@@ -1110,32 +1117,32 @@
         <f t="shared" si="0"/>
         <v>BE0</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>7</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
         <v>3</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="I9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="K9" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="3" t="str">
+      <c r="L9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 8, 'BE01', 'BE0', 7, 1, 3, BIOGAS, DRE345, N/A; </v>
-      </c>
-      <c r="O9" s="1"/>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 8, 'BE01', 'BE0','', 7, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
         <v>9</v>
       </c>
@@ -1146,32 +1153,32 @@
         <f t="shared" si="0"/>
         <v>BE0</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>8</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9">
         <v>2</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="I10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="K10" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="K10" s="3" t="str">
+      <c r="L10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 9, 'BE02', 'BE0', 8, 1, 2, BIOGAS, N/A, Oscar Flores; </v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 9, 'BE02', 'BE0','', 8, 1, 2, 'BIOGAS', 'N/A', 'Oscar Flores'; </v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B11" s="4">
         <v>11</v>
       </c>
@@ -1182,31 +1189,31 @@
         <f t="shared" si="0"/>
         <v>BE0</v>
       </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
         <v>3</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="I11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="K11" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K11" s="3" t="str">
+      <c r="L11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 11, 'BE05', 'BE0', 9, 1, 3, BIOGAS, ABC123, N/A; </v>
-      </c>
-      <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 11, 'BE05', 'BE0','', 9, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B12" s="4">
         <v>12</v>
       </c>
@@ -1217,35 +1224,35 @@
         <f t="shared" si="0"/>
         <v>BG0</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>10</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9">
         <v>3</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="I12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="K12" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K12" s="3" t="str">
+      <c r="L12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 12, 'BG02', 'BG0', 10, 1, 3, BIOGAS, BCD456, N/A; </v>
-      </c>
-      <c r="L12" s="2"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 12, 'BG02', 'BG0','', 10, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B13" s="4">
         <v>13</v>
       </c>
@@ -1256,31 +1263,31 @@
         <f t="shared" si="0"/>
         <v>BG0</v>
       </c>
-      <c r="E13">
-        <v>11</v>
-      </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="K13" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K13" s="3" t="str">
+      <c r="L13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 13, 'BG05', 'BG0', 11, 0, 1, BIOGAS, DRE345, N/A; </v>
-      </c>
-      <c r="P13" s="7"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 13, 'BG05', 'BG0','', 11, 0, 1, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B14" s="4">
         <v>14</v>
       </c>
@@ -1291,31 +1298,31 @@
         <f t="shared" si="0"/>
         <v>BG0</v>
       </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
       <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
         <v>3</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="K14" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K14" s="3" t="str">
+      <c r="L14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 14, 'BG06', 'BG0', 12, 1, 3, BIOGAS, EDF678, N/A; </v>
-      </c>
-      <c r="P14" s="7"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 14, 'BG06', 'BG0','', 12, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B15" s="4">
         <v>15</v>
       </c>
@@ -1326,31 +1333,31 @@
         <f t="shared" si="0"/>
         <v>BG0</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>13</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9">
         <v>2</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="K15" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="K15" s="3" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, ",B15,", '",C15,"', '",D15,"', ",E15,", ",F15,", ",G15,", '",H15,"', '",I15,"', '",J15,"'; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 15, 'BG08', 'BG0', 13, 1, 2, 'BIOGAS', 'N/A', 'Ejercito Nacional'; </v>
-      </c>
-      <c r="P15" s="7"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 15, 'BG08', 'BG0','', 13, 1, 2, 'BIOGAS', 'N/A', 'Ejercito Nacional'; </v>
+      </c>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B16" s="4">
         <v>16</v>
       </c>
@@ -1361,31 +1368,31 @@
         <f t="shared" si="0"/>
         <v>BG0</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>14</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9">
         <v>3</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="K16" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K16" s="3" t="str">
-        <f t="shared" ref="K16:K50" si="2">CONCATENATE("EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, ",B16,", '",C16,"', '",D16,"', ",E16,", ",F16,", ",G16,", '",H16,"', '",I16,"', '",J16,"'; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 16, 'BG09', 'BG0', 14, 0, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-      <c r="P16" s="7"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 16, 'BG09', 'BG0','', 14, 0, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17" s="4">
         <v>17</v>
       </c>
@@ -1396,31 +1403,31 @@
         <f t="shared" si="0"/>
         <v>BG1</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>15</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9">
         <v>3</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="K17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K17" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 17, 'BG10', 'BG1', 15, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-      <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 17, 'BG10', 'BG1','', 15, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="4">
         <v>18</v>
       </c>
@@ -1431,31 +1438,31 @@
         <f t="shared" si="0"/>
         <v>BG1</v>
       </c>
-      <c r="E18">
-        <v>16</v>
-      </c>
       <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9">
         <v>3</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="K18" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K18" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 18, 'BG11', 'BG1', 16, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L18" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 18, 'BG11', 'BG1','', 16, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19" s="4">
         <v>19</v>
       </c>
@@ -1466,31 +1473,31 @@
         <f t="shared" si="0"/>
         <v>BG1</v>
       </c>
-      <c r="E19">
-        <v>17</v>
-      </c>
       <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9">
+        <v>17</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="9">
         <v>3</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="K19" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K19" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 19, 'BG18', 'BG1', 17, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 19, 'BG18', 'BG1','', 17, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="4">
         <v>20</v>
       </c>
@@ -1501,31 +1508,31 @@
         <f t="shared" si="0"/>
         <v>BG1</v>
       </c>
-      <c r="E20">
-        <v>18</v>
-      </c>
       <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9">
+        <v>18</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="9">
         <v>2</v>
       </c>
-      <c r="H20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="K20" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 20, 'BG12', 'BG1', 18, 1, 2, 'BIOGAS', 'N/A', 'Paraje San Isidro'; </v>
-      </c>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 20, 'BG12', 'BG1','', 18, 1, 2, 'BIOGAS', 'N/A', 'Paraje San Isidro'; </v>
+      </c>
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21" s="4">
         <v>21</v>
       </c>
@@ -1536,31 +1543,31 @@
         <f t="shared" si="0"/>
         <v>BG1</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>19</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9">
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="9">
         <v>3</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="K21" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 21, 'BG19', 'BG1', 19, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 21, 'BG19', 'BG1','', 19, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22" s="4">
         <v>22</v>
       </c>
@@ -1571,31 +1578,31 @@
         <f t="shared" si="0"/>
         <v>BG2</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>20</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" s="9">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="9">
         <v>3</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="K22" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K22" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 22, 'BG20', 'BG2', 20, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-      <c r="P22" s="8"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 22, 'BG20', 'BG2','', 20, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B23" s="4">
         <v>23</v>
       </c>
@@ -1606,31 +1613,31 @@
         <f t="shared" si="0"/>
         <v>BG2</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>21</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" s="9">
-        <v>1</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="14" t="s">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="K23" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K23" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 23, 'BG21', 'BG2', 21, 0, 1, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 23, 'BG21', 'BG2','', 21, 0, 1, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24" s="4">
         <v>24</v>
       </c>
@@ -1641,31 +1648,31 @@
         <f t="shared" si="0"/>
         <v>BG2</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>22</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="9">
         <v>3</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="K24" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K24" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 24, 'BG22', 'BG2', 22, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 24, 'BG22', 'BG2','', 22, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25" s="4">
         <v>25</v>
       </c>
@@ -1676,31 +1683,31 @@
         <f t="shared" si="0"/>
         <v>BG2</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>23</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9">
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="9">
         <v>2</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="K25" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 25, 'BG27', 'BG2', 23, 1, 2, 'BIOGAS', 'N/A', 'Zaragoza'; </v>
-      </c>
-      <c r="P25" s="8"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 25, 'BG27', 'BG2','', 23, 1, 2, 'BIOGAS', 'N/A', 'Zaragoza'; </v>
+      </c>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="4">
         <v>26</v>
       </c>
@@ -1711,31 +1718,31 @@
         <f t="shared" si="0"/>
         <v>BG2</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>24</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
         <v>3</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="K26" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K26" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 26, 'BG28', 'BG2', 24, 0, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-      <c r="P26" s="8"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 26, 'BG28', 'BG2','', 24, 0, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B27" s="4">
         <v>27</v>
       </c>
@@ -1746,31 +1753,31 @@
         <f t="shared" si="0"/>
         <v>BG3</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>25</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="9">
         <v>3</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="K27" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K27" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 27, 'BG30', 'BG3', 25, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-      <c r="P27" s="8"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 27, 'BG30', 'BG3','', 25, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28" s="4">
         <v>28</v>
       </c>
@@ -1781,31 +1788,31 @@
         <f t="shared" si="0"/>
         <v>BG3</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>26</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9">
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="9">
         <v>3</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="K28" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K28" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 28, 'BG31', 'BG3', 26, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-      <c r="P28" s="8"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 28, 'BG31', 'BG3','', 26, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29" s="4">
         <v>29</v>
       </c>
@@ -1816,31 +1823,31 @@
         <f t="shared" si="0"/>
         <v>C13</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>27</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="9">
         <v>3</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="K29" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K29" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 29, 'C135', 'C13', 27, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-      <c r="P29" s="8"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 29, 'C135', 'C13','', 27, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30" s="4">
         <v>30</v>
       </c>
@@ -1851,31 +1858,31 @@
         <f t="shared" si="0"/>
         <v>U55</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>28</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9">
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="9">
         <v>2</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="K30" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K30" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 30, 'U55 EXP', 'U55', 28, 1, 2, 'BIOGAS', 'N/A', 'Av. Talamas camanadari'; </v>
-      </c>
-      <c r="P30" s="8"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 30, 'U55 EXP', 'U55','', 28, 1, 2, 'BIOGAS', 'N/A', 'Av. Talamas camanadari'; </v>
+      </c>
+      <c r="Q30" s="8"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B31" s="4">
         <v>31</v>
       </c>
@@ -1886,31 +1893,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>29</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9">
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="9">
         <v>3</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="K31" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K31" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 31, 'C121', 'C12', 29, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-      <c r="P31" s="8"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 31, 'C121', 'C12','', 29, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q31" s="8"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32" s="4">
         <v>32</v>
       </c>
@@ -1921,31 +1928,31 @@
         <f t="shared" si="0"/>
         <v>C13</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>30</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" s="9">
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="9">
         <v>3</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="K32" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K32" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 32, 'C132', 'C13', 30, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-      <c r="P32" s="8"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 32, 'C132', 'C13','', 30, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+      <c r="Q32" s="8"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33" s="4">
         <v>33</v>
       </c>
@@ -1956,31 +1963,31 @@
         <f t="shared" si="0"/>
         <v>C13</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>31</v>
       </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33" s="9">
-        <v>1</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="K33" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K33" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 33, 'C134', 'C13', 31, 0, 1, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-      <c r="P33" s="8"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 33, 'C134', 'C13','', 31, 0, 1, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="Q33" s="8"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B34" s="4">
         <v>34</v>
       </c>
@@ -1991,31 +1998,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>32</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9">
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="9">
         <v>3</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="K34" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K34" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 34, 'C122', 'C12', 32, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-      <c r="P34" s="8"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 34, 'C122', 'C12','', 32, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="Q34" s="8"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B35" s="4">
         <v>35</v>
       </c>
@@ -2026,31 +2033,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>33</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" s="9">
         <v>2</v>
       </c>
-      <c r="H35" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="K35" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="K35" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 35, 'C123', 'C12', 33, 1, 2, 'BIOGAS', 'N/A', 'Yepomera'; </v>
-      </c>
-      <c r="P35" s="8"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 35, 'C123', 'C12','', 33, 1, 2, 'BIOGAS', 'N/A', 'Yepomera'; </v>
+      </c>
+      <c r="Q35" s="8"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B36" s="4">
         <v>36</v>
       </c>
@@ -2061,31 +2068,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>34</v>
       </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36" s="9">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9">
         <v>3</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="K36" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 36, 'C124', 'C12', 34, 0, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-      <c r="P36" s="8"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L36" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 36, 'C124', 'C12','', 34, 0, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+      <c r="Q36" s="8"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B37" s="4">
         <v>37</v>
       </c>
@@ -2096,31 +2103,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>35</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" s="9">
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="9">
         <v>3</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="K37" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K37" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 37, 'C125', 'C12', 35, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-      <c r="P37" s="8"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 37, 'C125', 'C12','', 35, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B38" s="4">
         <v>38</v>
       </c>
@@ -2131,31 +2138,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>36</v>
       </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38" s="9">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="9">
         <v>3</v>
       </c>
-      <c r="H38" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="K38" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K38" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 38, 'C126', 'C12', 36, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-      <c r="P38" s="8"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L38" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 38, 'C126', 'C12','', 36, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+      <c r="Q38" s="8"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B39" s="4">
         <v>39</v>
       </c>
@@ -2166,31 +2173,31 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>37</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" s="9">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9">
         <v>3</v>
       </c>
-      <c r="H39" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J39" s="14" t="s">
+      <c r="K39" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 39, 'C127', 'C12', 37, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-      <c r="P39" s="8"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 39, 'C127', 'C12','', 37, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+      <c r="Q39" s="8"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B40" s="4">
         <v>40</v>
       </c>
@@ -2201,30 +2208,30 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>38</v>
       </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" s="9">
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" s="9">
         <v>2</v>
       </c>
-      <c r="H40" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="K40" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="K40" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 40, 'C128', 'C12', 38, 1, 2, 'BIOGAS', 'N/A', 'Henequen'; </v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L40" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 40, 'C128', 'C12','', 38, 1, 2, 'BIOGAS', 'N/A', 'Henequen'; </v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B41" s="4">
         <v>41</v>
       </c>
@@ -2235,30 +2242,30 @@
         <f t="shared" si="0"/>
         <v>C12</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>39</v>
       </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41" s="9">
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="9">
         <v>3</v>
       </c>
-      <c r="H41" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="K41" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K41" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 41, 'C129', 'C12', 39, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 41, 'C129', 'C12','', 39, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B42" s="4">
         <v>42</v>
       </c>
@@ -2269,30 +2276,30 @@
         <f t="shared" si="0"/>
         <v>C13</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>40</v>
       </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" s="9">
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9">
         <v>3</v>
       </c>
-      <c r="H42" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I42" s="14" t="s">
+      <c r="I42" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J42" s="14" t="s">
+      <c r="K42" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K42" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 42, 'C130', 'C13', 40, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 42, 'C130', 'C13','', 40, 1, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B43" s="4">
         <v>43</v>
       </c>
@@ -2303,30 +2310,30 @@
         <f t="shared" si="0"/>
         <v>C13</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>41</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43" s="9">
-        <v>1</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="14" t="s">
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" s="9">
+        <v>1</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J43" s="14" t="s">
+      <c r="K43" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 43, 'C131', 'C13', 41, 0, 1, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 43, 'C131', 'C13','', 41, 0, 1, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B44" s="4">
         <v>44</v>
       </c>
@@ -2337,30 +2344,30 @@
         <f t="shared" si="0"/>
         <v>C13</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>42</v>
       </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" s="9">
         <v>3</v>
       </c>
-      <c r="H44" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="K44" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K44" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 44, 'C136', 'C13', 42, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L44" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 44, 'C136', 'C13','', 42, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B45" s="4">
         <v>45</v>
       </c>
@@ -2371,30 +2378,30 @@
         <f t="shared" si="0"/>
         <v>C02</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>43</v>
       </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45" s="9">
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="9">
         <v>2</v>
       </c>
-      <c r="H45" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" s="14" t="s">
+      <c r="I45" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="K45" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="K45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 45, 'C02', 'C02', 43, 1, 2, 'BIOGAS', 'N/A', 'Av. Gomez Morin'; </v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L45" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 45, 'C02', 'C02','', 43, 1, 2, 'BIOGAS', 'N/A', 'Av. Gomez Morin'; </v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B46" s="4">
         <v>46</v>
       </c>
@@ -2405,30 +2412,30 @@
         <f t="shared" si="0"/>
         <v>C43</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>44</v>
       </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46" s="9">
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46" s="9">
         <v>3</v>
       </c>
-      <c r="H46" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" s="14" t="s">
+      <c r="I46" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J46" s="14" t="s">
+      <c r="K46" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 46, 'C43', 'C43', 44, 0, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L46" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 46, 'C43', 'C43','', 44, 0, 3, 'BIOGAS', 'EDF678', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B47" s="4">
         <v>47</v>
       </c>
@@ -2439,30 +2446,30 @@
         <f t="shared" si="0"/>
         <v>C11</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>45</v>
       </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9">
         <v>3</v>
       </c>
-      <c r="H47" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="14" t="s">
+      <c r="I47" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J47" s="14" t="s">
+      <c r="K47" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K47" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 47, 'C116', 'C11', 45, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="L47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 47, 'C116', 'C11','', 45, 1, 3, 'BIOGAS', 'ABC123', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B48" s="4">
         <v>48</v>
       </c>
@@ -2473,30 +2480,30 @@
         <f t="shared" si="0"/>
         <v>U02</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>46</v>
       </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" s="9">
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" s="9">
         <v>3</v>
       </c>
-      <c r="H48" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I48" s="14" t="s">
+      <c r="I48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="J48" s="14" t="s">
+      <c r="K48" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K48" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 48, 'U02', 'U02', 46, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="L48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 48, 'U02', 'U02','', 46, 1, 3, 'BIOGAS', 'BCD456', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B49" s="4">
         <v>49</v>
       </c>
@@ -2507,30 +2514,30 @@
         <f t="shared" si="0"/>
         <v>U46</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>47</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9">
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9">
         <v>3</v>
       </c>
-      <c r="H49" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I49" s="14" t="s">
+      <c r="I49" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J49" s="14" t="s">
+      <c r="K49" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K49" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 49, 'U46', 'U46', 47, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="L49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 49, 'U46', 'U46','', 47, 1, 3, 'BIOGAS', 'DRE345', 'N/A'; </v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B50" s="4">
         <v>50</v>
       </c>
@@ -2541,31 +2548,31 @@
         <f t="shared" si="0"/>
         <v>U53</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>48</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" s="9">
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="9">
         <v>2</v>
       </c>
-      <c r="H50" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" s="14" t="s">
+      <c r="I50" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="K50" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="K50" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PRODUCTO] 0,0, 50, 'U53', 'U53', 48, 1, 2, 'BIOGAS', 'N/A', 'Panamericana'; </v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="G51" s="9"/>
+      <c r="L50" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 50, 'U53', 'U53','', 48, 1, 2, 'BIOGAS', 'N/A', 'Panamericana'; </v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="H51" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>